<commit_message>
Added a note detailing a sample architecture.
Added notes in the spreadsheets comparing results between the tweaked model
and the original model.
</commit_message>
<xml_diff>
--- a/src/pytorch/results/High FC Numbers (240, 120)/Results - Larger FC Parameters.xlsx
+++ b/src/pytorch/results/High FC Numbers (240, 120)/Results - Larger FC Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc\Documents\CPS 803\Main Project\src\pytorch\results\High FC Numbers (240, 120)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D1A4D9-DA66-4292-8159-0EB1173F1208}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E27F02E-5124-490C-8330-E3CBC6D4D7C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="390" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Batch Size</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Epochs</t>
+  </si>
+  <si>
+    <t>No significant difference for the same batch sizes on the original model</t>
   </si>
 </sst>
 </file>
@@ -75,9 +78,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,7 +426,7 @@
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -456,7 +460,7 @@
         <v>0.92320000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -473,7 +477,7 @@
         <v>0.92669999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>16</v>
       </c>
@@ -490,17 +494,49 @@
         <v>0.85089999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A8:H8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>